<commit_message>
add run all datasets fix divide by zero
</commit_message>
<xml_diff>
--- a/results/left right based.xlsx
+++ b/results/left right based.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salmo\Desktop\AI-diagnosis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D46AB34-953D-4884-92A8-81B76CAA6163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130332C5-50B8-4660-AB41-DBFEBCDE6F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30195" yWindow="-4785" windowWidth="17280" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1116" yWindow="492" windowWidth="13824" windowHeight="7224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BJ$481</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2502,8 +2514,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BJ481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M458" workbookViewId="0">
-      <selection activeCell="H482" sqref="H482"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AW1" sqref="AW1:AW1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>